<commit_message>
adding more data files
</commit_message>
<xml_diff>
--- a/projectData.xlsx
+++ b/projectData.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chrdavi\Documents\transfer\Documents\pers\school\ETM640-Operations Research\final project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A5E6AE-A252-43E4-B7B4-E7236F364675}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE97C07-6B52-4D82-A470-E3326428FB3F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8778" xr2:uid="{7139B8BF-3992-4399-A030-7D8398AD96AE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8778" activeTab="3" xr2:uid="{7139B8BF-3992-4399-A030-7D8398AD96AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Home Configurations" sheetId="1" r:id="rId1"/>
-    <sheet name="Robot Info" sheetId="2" r:id="rId2"/>
+    <sheet name="Robot Info-old" sheetId="2" r:id="rId2"/>
+    <sheet name="Robot Info" sheetId="3" r:id="rId3"/>
+    <sheet name="Package Configs" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,6 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>Customer</t>
   </si>
@@ -112,16 +115,69 @@
   </si>
   <si>
     <t>1 minute per 2 sq/foot of window</t>
+  </si>
+  <si>
+    <t>Robot</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Package 1</t>
+  </si>
+  <si>
+    <t>Package 2</t>
+  </si>
+  <si>
+    <t>Package 3</t>
+  </si>
+  <si>
+    <t>Package 4</t>
+  </si>
+  <si>
+    <t>Package 5</t>
+  </si>
+  <si>
+    <t>Package 6</t>
+  </si>
+  <si>
+    <t>Robot 1</t>
+  </si>
+  <si>
+    <t>Robot 2</t>
+  </si>
+  <si>
+    <t>Robot 3</t>
+  </si>
+  <si>
+    <t>Robot 4</t>
+  </si>
+  <si>
+    <t>Robot 5</t>
+  </si>
+  <si>
+    <t>Profit</t>
+  </si>
+  <si>
+    <t>Available</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,14 +203,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -469,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B9B8EE-5CC8-4D45-AACA-DC34D763C90E}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -884,4 +943,285 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9874EE0-45F5-4C0C-AA47-9F5A6845A5B7}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="13.734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83984375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
+        <v>400</v>
+      </c>
+      <c r="D2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2">
+        <v>600</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2">
+        <v>500</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>300</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2">
+        <v>600</v>
+      </c>
+      <c r="D6">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F96F6B61-7950-4E47-93FB-E276B7CF1EE0}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="3" max="3" width="9.41796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>18</v>
+      </c>
+      <c r="E7">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>19</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>